<commit_message>
crawling 100% & processing 75%
</commit_message>
<xml_diff>
--- a/application/static/excel_data/data_crawling(13-11-2020).xlsx
+++ b/application/static/excel_data/data_crawling(13-11-2020).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -26,6 +26,56 @@
   </si>
   <si>
     <t>created_at</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>Satu keluarga di Jogja dinyatakan positif Covid-19.
+#pakaimasker      #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/vcU6dD0bMI</t>
+  </si>
+  <si>
+    <t>Seri Akhlak Anak Hebat;Nikmatnya Besabar - Diskon 20% menjadi Rp.28000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS: Hujan turun saat Gema dan Gina
+sedang bermain https://t.co/cWjd2xQ82U</t>
+  </si>
+  <si>
+    <t>Otw ujian semester, wish me luck
+#daring #belajardirumah</t>
+  </si>
+  <si>
+    <t>HARI INI PASIEN SEMBUH BERTAMBAH 14 ORANG, 10 KASUS BARU DAN 1 PROBABLE MENINGGAL
+INFORMASI LENGKAPNYA DI👉 https://t.co/B5YdjJM7g6
+#ayolawancorona #belajardirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak #pakemasker #tetapwaspada #coronabisasembuh https://t.co/2jj3oq2j3x</t>
+  </si>
+  <si>
+    <t>Update Perkembangan Covid-19 di Kabupaten Luwu Timur per 13 November 2020. 
+14 sembuh dan 10 kasus baru.
+Perbaharui terus informasi anda di https://t.co/D4pL3qgDlY
+#ayolawancorona #belajardirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak https://t.co/Ux1pGQCWlz</t>
+  </si>
+  <si>
+    <t>Di tikung sultan andara 😂
+#Mutualankuy #gempi #rafatar #elbarak #nikung #BelajarDirumah #follow #dirumahaja https://t.co/yFAvDMXgZI</t>
+  </si>
+  <si>
+    <t>Nabi Muhammad SAW Idolaku - Diskon 20% menjadi Rp.42400
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Assalamualaikum  Teman-Teman apakah kalian ingin masuk Surga https://t.co/pgoQruBpPm</t>
+  </si>
+  <si>
+    <t>SELURUH FRAKSI SEPAKATI PENYERTAAN MODAL KE BANK SULSELBAR
+BACA BERITA LENGKAPNYA DI 👉 https://t.co/1Ty1PIkena
+#ayolawancorona #belajardirumah #beribadahdirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak #pakemasker #tetapwaspada #coronabisasembuh https://t.co/EpO1YRYDme</t>
+  </si>
+  <si>
+    <t>IBI LUWU TIMUR GELAR MUSCAB IV MASA BAKTI 2018-2023
+BACA INFORMASI LENGKAPNYA DI 👉 https://t.co/nWiO9zSPMU
+#ayolawancorona #belajardirumah #beribadahdirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak #pakemasker #tetapwaspada #coronabisasembuh https://t.co/WcHc4Ws7tR</t>
   </si>
   <si>
     <t>Mengenal Allah Mencintai Islam A to Z - Diskon 20% menjadi Rp.64000
@@ -35,17 +85,462 @@
 Mengenal https://t.co/un20bP646U</t>
   </si>
   <si>
+    <t>Psikologi Pernikahan; Menyelami Rahasia Pernikahan - Diskon 20% menjadi Rp.48000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Buku ini wajib dimiliki oleh setiap https://t.co/UTf1p9FSnC</t>
+  </si>
+  <si>
+    <t>SEMANGAT DARING !
+#SEMANGATDARING
+#MakeAWish100M 
+Pagi-pagi 
+#Belajaryangtekun
+#belajardirumah https://t.co/ePjuTqwryf</t>
+  </si>
+  <si>
+    <t>Seri Metamorphosis:Nyam..Nyam Ulat lapar - Diskon 20% menjadi Rp.24000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Ada lho hewan yang berbeda ketika baru lahir dan https://t.co/DlwLCPPCmi</t>
+  </si>
+  <si>
+    <t>GELAR FGD, BAPELITBANGDA LUTIM PAPARKAN STRATEGI PENANGGULANGAN KEMISKINAN DAERAH
+LIHAT STATISTIK LENGKAPNYA DI 👉 https://t.co/QacEdjVi8G
+#ayolawancorona #belajardirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak #pakemasker #tetapwaspada #coronabisasembuh https://t.co/O4JZnb8Ret</t>
+  </si>
+  <si>
+    <t>DUKUNG TENAGA KESEHATAN, DWP LUWU TIMUR LAKUKAN GERAKAN TEPUK TANGAN 56 DETIK
+BACA INFOEMASI LENGKAPNYA 👉 https://t.co/sIeDouDBp4
+#ayolawancorona #belajardirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak #pakemasker #tetapwaspada #coronabisasembuh https://t.co/K2n3YJJce3</t>
+  </si>
+  <si>
+    <t>Satpol PP DIY menyiagakan ratusan personel guna memperketat pengawasan protokol kesehatan di Pasar Beringharjo.
+#pakaimasker     #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/vif1ASvPdU</t>
+  </si>
+  <si>
+    <t>Pemkot Yogyakarta menetapkan daerah Malioboro jadi kawasan tanpa rokok, Kamis (12/11/2020).
+#pakaimasker     #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/sVUIglbDxl</t>
+  </si>
+  <si>
+    <t>Kapanewon Banguntapan dan Sewon memberlakukan Pembatasan Sosial Berskala Kecil (PSBK).
+#pakaimasker     #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/JI1OLv1Ges</t>
+  </si>
+  <si>
+    <t>Penyebaran virus corona di Kabupaten Bantul, DIY, tercatat mengalami peningkatan drastis.
+#pakaimasker     #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/VWbmPr5SHf</t>
+  </si>
+  <si>
+    <t>Seri Metamorphosis:Ngiing...Ngiing...Nyamuk Terbang - Diskon 20% menjadi Rp.24000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Ada lho hewan yang
+bentuk nama dan https://t.co/AgPgeRnvFS</t>
+  </si>
+  <si>
+    <t>@INICLIPS adalah #ChannelYoutube yang membahas mengenai #perfilman, seperti :
+#AlurCeritaFilm #RangkumFilm #ReviewFilm #KomenFilm #RekomendasiFilm
+#SubscribeNow
+#AlurFilm
+#dirumahaja
+#kerjadirumahaja
+#belajardirumah
+#VirusCorona
+#COVID19indonesia</t>
+  </si>
+  <si>
+    <t>Seri Metamorphosis:Kecipak..Kecipuk...Katak Berenang - Diskon 20% menjadi Rp.24000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Ada lho hewan yang bentuk nama
+dan</t>
+  </si>
+  <si>
+    <t>Pandemi COVID-19 memunculkan beragam kebiasaan baru.
+#pakaimasker     #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/HbhMLkqx3d</t>
+  </si>
+  <si>
+    <t>Sultan berharap penerapan protokol kesehatan menjadi kebiasaan bagi masyarakat.
+#pakaimasker    #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/SeGtRYY4HX</t>
+  </si>
+  <si>
+    <t>Pasien Covid-19 di DIY bertambah sebanyak 79 kasus per Kamis
+#pakaimasker    #BelajardiRumah #COVID19 #COVID__19 #COVIDー19 #coronavirus #COVID #CoronaUpdate #Covid_19 #Corona #VirusCorona #updatecorona
+https://t.co/AWykuMAeFD</t>
+  </si>
+  <si>
+    <t>Nabi Muhammad SAW Idolaku - Diskon 20% menjadi Rp.42400
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Assalamualaikum  Teman-Teman apakah kalian ingin masuk Surga https://t.co/pXS3GNEe4q</t>
+  </si>
+  <si>
+    <t>PJS. BUPATI LUTIM APRESIASI PROGRAM KSWP OPTIMALKAN POTENSI PAJAK
+BACA INFORMASI LENGKAPNYA DI 👉 https://t.co/3S86DWHjIP
+#ayolawancorona #belajardirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak #pakemasker #tetapwaspada #coronabisasembuh https://t.co/22CYnG5xRy</t>
+  </si>
+  <si>
+    <t>https://t.co/doQkhRuar1
+Utk anak2 Paud yg hebat,  smg bisa menjadi bekal belajar yg menyenangkan dan bermanfaat. 💚💚💚
+#anakpaud 
+#anaktk 
+#belajardirumah 
+#belajaronline 
+#belajarjarakjauh https://t.co/gsDiIvdKsj</t>
+  </si>
+  <si>
+    <t>Mengenal Allah Mencintai Islam A to Z - Diskon 20% menjadi Rp.64000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Assalamu`alaikum Teman-Teman ….
+Mengenal https://t.co/8Zo3CJgSyb</t>
+  </si>
+  <si>
+    <t>PASIEN SEMBUH MENINGKAT MENJADI 1.590 DAN 1 KASUS BARU HARI INI
+INFORMASI LENGKAPNYA BACA DI 👉 https://t.co/bJLtZZHUhU
+#ayolawancorona #belajardirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak #pakemasker #tetapwaspada #coronabisasembuh https://t.co/3YSGxkRa07</t>
+  </si>
+  <si>
+    <t>Update Perkembangan Covid-19 di Kabupaten Luwu Timur per 12 November 2020.
+13 sembuh dan 1 kasus baru.
+Perbaharui terus informasi anda di https://t.co/D4pL3qgDlY
+#ayolawancorona #belajardirumah #bermaindirumah #dirumahsaja #jagakebersihan #jagakesehatan #jagajarak https://t.co/ED73Tk77vL</t>
+  </si>
+  <si>
+    <t>#Yok belajar yookkk #belajardirumah #gerakan56detik https://t.co/n1RGeGAVKB</t>
+  </si>
+  <si>
+    <t>AN : Aktual,Hangat dan Menyengat https://t.co/ghZl6Fq9g0  #belajardirumah #asesmennasional @Pusmenjar</t>
+  </si>
+  <si>
+    <t>Seri Adab Berteman - Diskon 20% menjadi Rp.20000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Ima heran mengapa Puti tampak meminta uang kepada teman – temanya. https://t.co/eF4AQWbmsv</t>
+  </si>
+  <si>
+    <t>Seri Adab di Masjid - Diskon 20% menjadi Rp.20000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Abi bawa apa itu? tanya Ibu. Tidak biasanya Abi berangkat shalat https://t.co/YlYrePjyT1</t>
+  </si>
+  <si>
+    <t>Kamu bisa dapetin Bantuan Kuota Data Internet di nomor IM3 Ooredoo untuk #belajardirumah! Gak perlu ganti nomor, pastikan nomormu udah terdaftar di sekolah/kampusmu.
+Cek status kuota di myIM3 dan ikuti Kuis Pintar untuk menangin voucher belanja!
+Info 👉🏻 https://t.co/xHmXakVwA8 https://t.co/0M7lX5o1DP</t>
+  </si>
+  <si>
+    <t>Selamat Hari Ayah Nasional
+"Terima kasih, Ayah. Terima kasih."
+#kelaskita #carabarubelajarseru #belajardirumah
+#elearning #belajaronline #dirumahaja #HariAyah #HariAyahNasional https://t.co/1udOTmnQqk</t>
+  </si>
+  <si>
+    <t>Psikologi Pernikahan; Menyelami Rahasia Pernikahan - Diskon 20% menjadi Rp.48000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Buku ini wajib dimiliki oleh setiap https://t.co/d2O98NHt1F</t>
+  </si>
+  <si>
+    <t>Ini yang paling penting! Harus pinter pilah informasi biar gak kepikiran yang macem-macem :'(
+#kelaskita #carabarubelajarseru #belajardirumah
+#elearning #belajaronline #dirumahaja #harikesehatannasional https://t.co/01cIk3nK4A</t>
+  </si>
+  <si>
+    <t>Pastiin pola makan kita 4 sehat 5 semfurna~ 
+Tidur juga yang cukup, bicoz kalo begadang percuma skincare-nya lop.
+#kelaskita #carabarubelajarseru #belajardirumah
+#elearning #belajaronline #dirumahaja #harikesehatannasional https://t.co/tPKjDx5uxC</t>
+  </si>
+  <si>
+    <t>Yang hobinya rebahan gapapa, yang penting pikiran seger. Jangan lupa, kalo ada rezeki lebih boleh dong bantu-bantu yang membutuhkan.
+#kelaskita #carabarubelajarseru #belajardirumah
+#elearning #belajaronline #dirumahaja #harikesehatannasional https://t.co/UcyCwI8957</t>
+  </si>
+  <si>
+    <t>Olahraga itu perlu banget. Abis olahraga, ngobrol deh sama orang-orang tersayang. Dijamin capeknya langsung ilang!
+#kelaskita #carabarubelajarseru #belajardirumah
+#elearning #belajaronline #dirumahaja #harikesehatannasional https://t.co/ihnTZCC6vm</t>
+  </si>
+  <si>
+    <t>Di Hari Kesehatan Nasional ini, Kelaskita mau ajak kalian buat melakukan ritual wajib biar kesehatan mentalnya terjaga. Simak, yuk thread-nya!
+#kelaskita #carabarubelajarseru #belajardirumah
+ #elearning #belajaronline #dirumahaja #harikesehatannasional https://t.co/35vHLTAyOt</t>
+  </si>
+  <si>
+    <t>Selamat Hari Kesehatan Nasional!
+Jaga diri, keluarga, dan masyarakat. Selamatkan bangsa dari pandemi Covid-19.
+#kelaskita #carabarubelajarseru #belajardirumah
+#elearning #belajaronline #dirumahaja #harikesehatannasional #covid19 https://t.co/Xm4Qv6nFb8</t>
+  </si>
+  <si>
+    <t>Ghisa dan tugas belajar dirumah nya.
+#belajardirumah #AnakSekolah #YouTubeDOWN https://t.co/uIOfOk9nsc</t>
+  </si>
+  <si>
+    <t>Sedang butuh menghapus banyak baris, kolom, atau cell secara cepat? Segera sorot baris, kolom, atau cellmu tersebut dan tekan Ctrl + - (Command + - pada Mac)
+#belajardirumah #tipsexcel #computeexpert</t>
+  </si>
+  <si>
+    <t>🌵•FOKUS BELAJAR•🌵
+[A Thread]
+#studytwt #STUDY #studygram #studytip #studytips #belajardirumah #belajar #fokus #tips #info #studying #like</t>
+  </si>
+  <si>
+    <t>Temukan BUKU PETUNJUK GURU 123 (3 Buku) Matematika Gasing dengan potongan 50%! Hanya Rp50.000. Dapatkan sekarang juga di Shopee! https://t.co/QEngPVywh5
+#Matemtika
+#matematika 
+#MATEMATICA 
+#matematicasparaprogres 
+#Bukumurah
+#tematik
+#NKRITetaplahMajuMelangkah 
+#belajardirumah https://t.co/YOA7ajAFoV</t>
+  </si>
+  <si>
+    <t>PPKN KELAS 7 - FAKTOR PENYEBAB KEBERAGAMAN DI INDONESIA (BAB 4 - PART 1) https://t.co/WDw1zGK1MV lewat @YouTube 
+#pkn2020 #belajardirumah #ppkn #sekolah #ppkn</t>
+  </si>
+  <si>
+    <t>Seri Adab Bersuci - Diskon 20% menjadi Rp.20000
+Gratis ongkos kirim hingga 40rb keseluruh Indonesia.
+#mainanbukuanak #promo #dirumahaja #belajardirumah #buku #membaca #booklover #bookstorm  
+SINOPSIS:Sena kesal sekali. Ia tak sengaja sengaja menginjak kotoran ayam saat https://t.co/mPL3vk53RV</t>
+  </si>
+  <si>
+    <t>Jalani hari hari mu, atur lagi target mu, ingatin lagi dirimu bahwa kamu harus sukses dan tetap positif #positive #belajardirumah #Target #goals #pikiran #semangat</t>
+  </si>
+  <si>
+    <t>ayoyogyacom</t>
+  </si>
+  <si>
     <t>mainanbukuanak</t>
   </si>
   <si>
+    <t>YonathanElbert</t>
+  </si>
+  <si>
+    <t>diskominfolutim</t>
+  </si>
+  <si>
+    <t>alamsyah05</t>
+  </si>
+  <si>
+    <t>Sririzkikiii</t>
+  </si>
+  <si>
+    <t>iniclips</t>
+  </si>
+  <si>
+    <t>MyAbee_Gabriel</t>
+  </si>
+  <si>
+    <t>RegianNaza</t>
+  </si>
+  <si>
+    <t>onesmmat</t>
+  </si>
+  <si>
+    <t>IM3Ooredoo</t>
+  </si>
+  <si>
+    <t>kelaskitadotcom</t>
+  </si>
+  <si>
+    <t>BukanAr01743087</t>
+  </si>
+  <si>
+    <t>expert_compute</t>
+  </si>
+  <si>
+    <t>Babyupii2</t>
+  </si>
+  <si>
+    <t>gasing67038183</t>
+  </si>
+  <si>
+    <t>Widiakww</t>
+  </si>
+  <si>
+    <t>RusaliAdam</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 12:36:23 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 11:36:07 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 11:07:23 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 10:58:39 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 10:54:06 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 10:18:54 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 08:38:16 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 07:09:36 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 06:28:24 +0000 2020</t>
+  </si>
+  <si>
     <t>Fri Nov 13 05:37:55 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 02:36:16 +0000 2020</t>
+  </si>
+  <si>
+    <t>Fri Nov 13 01:57:11 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 23:37:31 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 22:35:06 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 22:17:49 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 21:25:35 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 21:24:32 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 21:23:39 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 21:22:48 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 20:39:51 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 19:21:21 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 19:21:08 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 19:18:47 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 19:18:29 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 19:18:16 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 17:37:54 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 15:58:25 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 15:55:51 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 15:39:37 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 14:39:27 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 13:09:53 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 13:09:14 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 11:47:33 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 10:43:51 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 10:39:09 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 10:29:35 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 09:29:22 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 08:37:09 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 08:36:11 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 08:00:16 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 06:12:24 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 05:37:47 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 05:09:29 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 05:08:03 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 05:05:41 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 05:03:56 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 05:02:12 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 04:45:40 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 04:08:03 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 03:15:50 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 03:03:53 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 02:55:39 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 02:46:23 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 02:36:08 +0000 2020</t>
+  </si>
+  <si>
+    <t>Thu Nov 12 00:41:29 +0000 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +555,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,16 +596,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,13 +904,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,22 +923,949 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
+        <v>1.327228816381473E+18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1.327213649421713E+18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1.327206419704074E+18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1.327204223671435E+18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>1.327203078198596E+18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>1.327194218557698E+18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1.327168894348345E+18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>1.327146579468423E+18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>1.327136209827721E+18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
         <v>1.327123505331266E+18</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>1.327077792882651E+18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>1.327067957013348E+18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>1.327032807466562E+18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>1.327017100804649E+18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>1.327012754096411E+18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>1.326999609269318E+18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>1.32699934410546E+18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>1.326999122642014E+18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>1.326998908824797E+18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>1.326988096764735E+18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>1.32696834224298E+18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>1.326968289684165E+18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>1.326967696722813E+18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>1.326967619581174E+18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>1.326967565965537E+18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>1.326942308298711E+18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>1.326917272477315E+18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>1.326916626609005E+18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>1.326912543416267E+18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>1.326897400590569E+18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>1.32687485944023E+18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>1.326874697879839E+18</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>1.326854140488634E+18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>1.326838108420149E+18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>1.326836928633696E+18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>1.326834518871867E+18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>1.326819367007347E+18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>1.32680622489815E+18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>1.326805982626771E+18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>1.326796943666844E+18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>1.326769796717875E+18</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>1.326761086301966E+18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>1.326753963882942E+18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>1.326753603239903E+18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>1.326753006340071E+18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>1.326752568232456E+18</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>1.326752130321953E+18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>1.326747971459822E+18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>1.326738503338611E+18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>1.326725362756198E+18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>1.326722355435983E+18</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>124</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>1.32672028190208E+18</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>1.326717952234672E+18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>1.326715370711904E+18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" t="s">
+        <v>127</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>1.326686520959402E+18</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B33" r:id="rId1" location="anakpaud%20&#10;#anaktk%20&#10;#belajardirumah%20&#10;#belajaronline%20&#10;#belajarjarakjauh%20https://t.co/gsDiIvdKsj"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>